<commit_message>
i don't even know
</commit_message>
<xml_diff>
--- a/data-raw/dac_exchange_day_a.xlsx
+++ b/data-raw/dac_exchange_day_a.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\R\misc_figures\data-raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vgz813\Desktop\R\misc_figures\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18A2B8BC-18E8-4E0A-AD2C-A15996ED12F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47D99EA9-E38F-46F2-8D40-DAAD59876783}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28695" yWindow="0" windowWidth="29010" windowHeight="23385" xr2:uid="{49542F80-B68A-47D4-9929-7FF12213D34E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{49542F80-B68A-47D4-9929-7FF12213D34E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
   <si>
     <t>id</t>
   </si>
@@ -165,6 +165,84 @@
   </si>
   <si>
     <t>Glu_v_T4_5</t>
+  </si>
+  <si>
+    <t>Hct_a_TTE</t>
+  </si>
+  <si>
+    <t>Hct_v_TTE</t>
+  </si>
+  <si>
+    <t>Hct_a_R1</t>
+  </si>
+  <si>
+    <t>Hct_v_R1</t>
+  </si>
+  <si>
+    <t>Hct_a_R2</t>
+  </si>
+  <si>
+    <t>Hct_v_R2</t>
+  </si>
+  <si>
+    <t>Hct_a_R3</t>
+  </si>
+  <si>
+    <t>Hct_v_R3</t>
+  </si>
+  <si>
+    <t>Hct_a_R5</t>
+  </si>
+  <si>
+    <t>Hct_v_R5</t>
+  </si>
+  <si>
+    <t>Hct_a_R10</t>
+  </si>
+  <si>
+    <t>Hct_v_R10</t>
+  </si>
+  <si>
+    <t>Hct_v_T15</t>
+  </si>
+  <si>
+    <t>Hct_a_T15</t>
+  </si>
+  <si>
+    <t>Hct_a_T0</t>
+  </si>
+  <si>
+    <t>Hct_v_T0</t>
+  </si>
+  <si>
+    <t>Hct_a_T0_5</t>
+  </si>
+  <si>
+    <t>Hct_v_T0_5</t>
+  </si>
+  <si>
+    <t>Hct_a_T1_5</t>
+  </si>
+  <si>
+    <t>Hct_v_T1_5</t>
+  </si>
+  <si>
+    <t>Hct_a_T2_5</t>
+  </si>
+  <si>
+    <t>Hct_v_T2_5</t>
+  </si>
+  <si>
+    <t>Hct_a_T3_5</t>
+  </si>
+  <si>
+    <t>Hct_v_T3_5</t>
+  </si>
+  <si>
+    <t>Hct_a_T4_5</t>
+  </si>
+  <si>
+    <t>Hct_v_T4_5</t>
   </si>
 </sst>
 </file>
@@ -213,7 +291,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -274,11 +352,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -306,11 +410,28 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -640,10 +761,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E41A862F-0CAF-4C8B-A1CF-BD1CDCF404B3}">
-  <dimension ref="A1:AQ20"/>
+  <dimension ref="A1:BQ22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="R18" sqref="R18"/>
+    <sheetView tabSelected="1" topLeftCell="AF1" workbookViewId="0">
+      <selection activeCell="BE22" sqref="AS21:BE22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -651,7 +772,7 @@
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -781,8 +902,86 @@
       <c r="AQ1" t="s">
         <v>28</v>
       </c>
+      <c r="AR1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AZ1" t="s">
+        <v>63</v>
+      </c>
+      <c r="BA1" t="s">
+        <v>64</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>65</v>
+      </c>
+      <c r="BC1" t="s">
+        <v>66</v>
+      </c>
+      <c r="BD1" t="s">
+        <v>67</v>
+      </c>
+      <c r="BE1" t="s">
+        <v>68</v>
+      </c>
+      <c r="BF1" t="s">
+        <v>43</v>
+      </c>
+      <c r="BG1" t="s">
+        <v>44</v>
+      </c>
+      <c r="BH1" t="s">
+        <v>45</v>
+      </c>
+      <c r="BI1" t="s">
+        <v>46</v>
+      </c>
+      <c r="BJ1" t="s">
+        <v>47</v>
+      </c>
+      <c r="BK1" t="s">
+        <v>48</v>
+      </c>
+      <c r="BL1" t="s">
+        <v>49</v>
+      </c>
+      <c r="BM1" t="s">
+        <v>50</v>
+      </c>
+      <c r="BN1" t="s">
+        <v>51</v>
+      </c>
+      <c r="BO1" t="s">
+        <v>52</v>
+      </c>
+      <c r="BP1" t="s">
+        <v>53</v>
+      </c>
+      <c r="BQ1" t="s">
+        <v>54</v>
+      </c>
     </row>
-    <row r="2" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -894,8 +1093,74 @@
       <c r="AQ2">
         <v>4.5</v>
       </c>
+      <c r="AR2">
+        <v>44.3</v>
+      </c>
+      <c r="AS2">
+        <v>46.6</v>
+      </c>
+      <c r="AT2">
+        <v>44.6</v>
+      </c>
+      <c r="AU2">
+        <v>46.8</v>
+      </c>
+      <c r="AV2">
+        <v>46.1</v>
+      </c>
+      <c r="AW2">
+        <v>46.8</v>
+      </c>
+      <c r="AX2">
+        <v>47.7</v>
+      </c>
+      <c r="AY2">
+        <v>48.3</v>
+      </c>
+      <c r="AZ2">
+        <v>48.2</v>
+      </c>
+      <c r="BA2">
+        <v>50.2</v>
+      </c>
+      <c r="BF2">
+        <v>48.9</v>
+      </c>
+      <c r="BG2">
+        <v>45.7</v>
+      </c>
+      <c r="BH2">
+        <v>47.9</v>
+      </c>
+      <c r="BI2">
+        <v>48.6</v>
+      </c>
+      <c r="BJ2">
+        <v>47.8</v>
+      </c>
+      <c r="BK2">
+        <v>48.1</v>
+      </c>
+      <c r="BL2">
+        <v>47.9</v>
+      </c>
+      <c r="BM2">
+        <v>50</v>
+      </c>
+      <c r="BN2">
+        <v>48.3</v>
+      </c>
+      <c r="BO2">
+        <v>50.4</v>
+      </c>
+      <c r="BP2">
+        <v>44.9</v>
+      </c>
+      <c r="BQ2">
+        <v>49</v>
+      </c>
     </row>
-    <row r="3" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>1</v>
       </c>
@@ -1025,8 +1290,86 @@
       <c r="AQ3">
         <v>3.7</v>
       </c>
+      <c r="AR3">
+        <v>41</v>
+      </c>
+      <c r="AS3">
+        <v>42</v>
+      </c>
+      <c r="AT3">
+        <v>43.7</v>
+      </c>
+      <c r="AU3">
+        <v>43.2</v>
+      </c>
+      <c r="AV3">
+        <v>44.4</v>
+      </c>
+      <c r="AW3">
+        <v>47.1</v>
+      </c>
+      <c r="AX3">
+        <v>47.1</v>
+      </c>
+      <c r="AY3">
+        <v>47.9</v>
+      </c>
+      <c r="AZ3">
+        <v>48.8</v>
+      </c>
+      <c r="BA3">
+        <v>48.1</v>
+      </c>
+      <c r="BB3">
+        <v>48.2</v>
+      </c>
+      <c r="BC3">
+        <v>47</v>
+      </c>
+      <c r="BD3">
+        <v>47.1</v>
+      </c>
+      <c r="BE3">
+        <v>50</v>
+      </c>
+      <c r="BF3">
+        <v>47.4</v>
+      </c>
+      <c r="BG3">
+        <v>48.3</v>
+      </c>
+      <c r="BH3">
+        <v>47</v>
+      </c>
+      <c r="BI3">
+        <v>45.3</v>
+      </c>
+      <c r="BJ3">
+        <v>44.8</v>
+      </c>
+      <c r="BK3">
+        <v>47.8</v>
+      </c>
+      <c r="BL3">
+        <v>50.5</v>
+      </c>
+      <c r="BM3">
+        <v>49.7</v>
+      </c>
+      <c r="BN3">
+        <v>50.8</v>
+      </c>
+      <c r="BO3">
+        <v>51.9</v>
+      </c>
+      <c r="BP3">
+        <v>51.1</v>
+      </c>
+      <c r="BQ3">
+        <v>49.6</v>
+      </c>
     </row>
-    <row r="4" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -1141,8 +1484,74 @@
       <c r="AQ4">
         <v>5.4</v>
       </c>
+      <c r="AR4">
+        <v>42.4</v>
+      </c>
+      <c r="AS4">
+        <v>42</v>
+      </c>
+      <c r="AT4">
+        <v>41.1</v>
+      </c>
+      <c r="AU4">
+        <v>44</v>
+      </c>
+      <c r="AV4">
+        <v>43.9</v>
+      </c>
+      <c r="AW4">
+        <v>44.7</v>
+      </c>
+      <c r="AX4">
+        <v>43.6</v>
+      </c>
+      <c r="AY4">
+        <v>46.1</v>
+      </c>
+      <c r="AZ4">
+        <v>46.3</v>
+      </c>
+      <c r="BA4">
+        <v>46.5</v>
+      </c>
+      <c r="BF4">
+        <v>46.6</v>
+      </c>
+      <c r="BG4">
+        <v>47.1</v>
+      </c>
+      <c r="BH4">
+        <v>48.507689566676945</v>
+      </c>
+      <c r="BI4">
+        <v>48.427677247181421</v>
+      </c>
+      <c r="BJ4">
+        <v>47.252363156822469</v>
+      </c>
+      <c r="BK4">
+        <v>49.186193452218888</v>
+      </c>
+      <c r="BL4">
+        <v>47.95546468664422</v>
+      </c>
+      <c r="BM4">
+        <v>49.075335023460013</v>
+      </c>
+      <c r="BN4">
+        <v>43.9</v>
+      </c>
+      <c r="BO4">
+        <v>45.1</v>
+      </c>
+      <c r="BP4">
+        <v>44.8</v>
+      </c>
+      <c r="BQ4">
+        <v>43.5</v>
+      </c>
     </row>
-    <row r="5" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>2</v>
       </c>
@@ -1263,8 +1672,80 @@
       <c r="AQ5">
         <v>4</v>
       </c>
+      <c r="AR5">
+        <v>40.6</v>
+      </c>
+      <c r="AS5">
+        <v>39.9</v>
+      </c>
+      <c r="AT5">
+        <v>43.3</v>
+      </c>
+      <c r="AU5">
+        <v>43.8</v>
+      </c>
+      <c r="AV5">
+        <v>43.3</v>
+      </c>
+      <c r="AW5">
+        <v>45.7</v>
+      </c>
+      <c r="AX5">
+        <v>46.4</v>
+      </c>
+      <c r="AY5">
+        <v>45.6</v>
+      </c>
+      <c r="AZ5">
+        <v>46.9</v>
+      </c>
+      <c r="BA5">
+        <v>46.9</v>
+      </c>
+      <c r="BB5">
+        <v>45.4</v>
+      </c>
+      <c r="BC5">
+        <v>46</v>
+      </c>
+      <c r="BF5">
+        <v>48.2</v>
+      </c>
+      <c r="BG5">
+        <v>45.8</v>
+      </c>
+      <c r="BH5">
+        <v>47.4</v>
+      </c>
+      <c r="BI5">
+        <v>46.8</v>
+      </c>
+      <c r="BJ5">
+        <v>44.4</v>
+      </c>
+      <c r="BK5">
+        <v>45.2</v>
+      </c>
+      <c r="BL5">
+        <v>44.8</v>
+      </c>
+      <c r="BM5">
+        <v>45.7</v>
+      </c>
+      <c r="BN5">
+        <v>45</v>
+      </c>
+      <c r="BO5">
+        <v>45.8</v>
+      </c>
+      <c r="BP5">
+        <v>40.299999999999997</v>
+      </c>
+      <c r="BQ5">
+        <v>42.4</v>
+      </c>
     </row>
-    <row r="6" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>3</v>
       </c>
@@ -1382,8 +1863,80 @@
       <c r="AQ6">
         <v>5.0902857290885715</v>
       </c>
+      <c r="AR6">
+        <v>45.1</v>
+      </c>
+      <c r="AS6">
+        <v>45.6</v>
+      </c>
+      <c r="AT6">
+        <v>45.1</v>
+      </c>
+      <c r="AU6">
+        <v>44.2</v>
+      </c>
+      <c r="AV6">
+        <v>42.7</v>
+      </c>
+      <c r="AW6">
+        <v>43.6</v>
+      </c>
+      <c r="AX6">
+        <v>47.9</v>
+      </c>
+      <c r="AY6">
+        <v>44.9</v>
+      </c>
+      <c r="AZ6">
+        <v>46.9</v>
+      </c>
+      <c r="BA6">
+        <v>50.5</v>
+      </c>
+      <c r="BB6">
+        <v>47.3</v>
+      </c>
+      <c r="BC6">
+        <v>47.5</v>
+      </c>
+      <c r="BF6">
+        <v>48.5</v>
+      </c>
+      <c r="BG6">
+        <v>47.6</v>
+      </c>
+      <c r="BH6">
+        <v>50</v>
+      </c>
+      <c r="BI6">
+        <v>48.2</v>
+      </c>
+      <c r="BJ6">
+        <v>48.9</v>
+      </c>
+      <c r="BK6">
+        <v>50.7</v>
+      </c>
+      <c r="BL6">
+        <v>47.6</v>
+      </c>
+      <c r="BM6">
+        <v>45.4</v>
+      </c>
+      <c r="BN6">
+        <v>46.7</v>
+      </c>
+      <c r="BO6">
+        <v>49.1</v>
+      </c>
+      <c r="BP6">
+        <v>45.919483783876444</v>
+      </c>
+      <c r="BQ6">
+        <v>45.274446272947955</v>
+      </c>
     </row>
-    <row r="7" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>3</v>
       </c>
@@ -1504,8 +2057,80 @@
       <c r="AQ7">
         <v>4.5</v>
       </c>
+      <c r="AR7">
+        <v>43.1</v>
+      </c>
+      <c r="AS7">
+        <v>36.4</v>
+      </c>
+      <c r="AT7">
+        <v>42.9</v>
+      </c>
+      <c r="AU7">
+        <v>42.2</v>
+      </c>
+      <c r="AV7">
+        <v>47</v>
+      </c>
+      <c r="AW7">
+        <v>47.7</v>
+      </c>
+      <c r="AX7">
+        <v>47.6</v>
+      </c>
+      <c r="AY7">
+        <v>48.8</v>
+      </c>
+      <c r="AZ7">
+        <v>49.8</v>
+      </c>
+      <c r="BA7">
+        <v>46.8</v>
+      </c>
+      <c r="BB7">
+        <v>45.3</v>
+      </c>
+      <c r="BC7">
+        <v>47.5</v>
+      </c>
+      <c r="BF7">
+        <v>50.3</v>
+      </c>
+      <c r="BG7">
+        <v>49.1</v>
+      </c>
+      <c r="BH7">
+        <v>50.4</v>
+      </c>
+      <c r="BI7">
+        <v>50.7</v>
+      </c>
+      <c r="BJ7">
+        <v>48.8</v>
+      </c>
+      <c r="BK7">
+        <v>49.6</v>
+      </c>
+      <c r="BL7">
+        <v>50</v>
+      </c>
+      <c r="BM7">
+        <v>46</v>
+      </c>
+      <c r="BN7">
+        <v>45.8</v>
+      </c>
+      <c r="BO7">
+        <v>46</v>
+      </c>
+      <c r="BP7">
+        <v>47.9</v>
+      </c>
+      <c r="BQ7">
+        <v>45.9</v>
+      </c>
     </row>
-    <row r="8" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>5</v>
       </c>
@@ -1608,8 +2233,68 @@
       <c r="AQ8">
         <v>6</v>
       </c>
+      <c r="AR8">
+        <v>44.7</v>
+      </c>
+      <c r="AS8">
+        <v>41.6</v>
+      </c>
+      <c r="AT8">
+        <v>46.2</v>
+      </c>
+      <c r="AU8">
+        <v>47.8</v>
+      </c>
+      <c r="AV8">
+        <v>49.5</v>
+      </c>
+      <c r="AW8">
+        <v>48.4</v>
+      </c>
+      <c r="AX8">
+        <v>50.7</v>
+      </c>
+      <c r="AY8">
+        <v>52.3</v>
+      </c>
+      <c r="BF8">
+        <v>48.5</v>
+      </c>
+      <c r="BG8">
+        <v>53.6</v>
+      </c>
+      <c r="BH8">
+        <v>51.1</v>
+      </c>
+      <c r="BI8">
+        <v>52.5</v>
+      </c>
+      <c r="BJ8">
+        <v>48.5</v>
+      </c>
+      <c r="BK8">
+        <v>51.8</v>
+      </c>
+      <c r="BL8">
+        <v>49.5</v>
+      </c>
+      <c r="BM8">
+        <v>52.8</v>
+      </c>
+      <c r="BN8">
+        <v>49.1</v>
+      </c>
+      <c r="BO8">
+        <v>50.5</v>
+      </c>
+      <c r="BP8">
+        <v>48.7</v>
+      </c>
+      <c r="BQ8">
+        <v>53</v>
+      </c>
     </row>
-    <row r="9" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>5</v>
       </c>
@@ -1721,8 +2406,74 @@
       <c r="AQ9">
         <v>5.0999999999999996</v>
       </c>
+      <c r="AR9">
+        <v>44</v>
+      </c>
+      <c r="AS9">
+        <v>41.8</v>
+      </c>
+      <c r="AT9">
+        <v>44.7</v>
+      </c>
+      <c r="AU9">
+        <v>43.7</v>
+      </c>
+      <c r="AV9">
+        <v>46.5</v>
+      </c>
+      <c r="AW9">
+        <v>46.5</v>
+      </c>
+      <c r="AX9">
+        <v>47.4</v>
+      </c>
+      <c r="AY9">
+        <v>47.6</v>
+      </c>
+      <c r="AZ9">
+        <v>49.1</v>
+      </c>
+      <c r="BA9">
+        <v>52.4</v>
+      </c>
+      <c r="BF9">
+        <v>50.3</v>
+      </c>
+      <c r="BG9">
+        <v>50.7</v>
+      </c>
+      <c r="BH9">
+        <v>48.9</v>
+      </c>
+      <c r="BI9">
+        <v>47.4</v>
+      </c>
+      <c r="BJ9">
+        <v>47.8</v>
+      </c>
+      <c r="BK9">
+        <v>44.1</v>
+      </c>
+      <c r="BL9">
+        <v>48.6</v>
+      </c>
+      <c r="BM9">
+        <v>47.8</v>
+      </c>
+      <c r="BN9">
+        <v>47.7</v>
+      </c>
+      <c r="BO9">
+        <v>49</v>
+      </c>
+      <c r="BP9">
+        <v>48.8</v>
+      </c>
+      <c r="BQ9">
+        <v>47.5</v>
+      </c>
     </row>
-    <row r="10" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>6</v>
       </c>
@@ -1825,8 +2576,68 @@
       <c r="AQ10">
         <v>4.8</v>
       </c>
+      <c r="AR10">
+        <v>45</v>
+      </c>
+      <c r="AS10">
+        <v>47.7</v>
+      </c>
+      <c r="AT10">
+        <v>47.5</v>
+      </c>
+      <c r="AU10">
+        <v>48.7</v>
+      </c>
+      <c r="AV10">
+        <v>48.5</v>
+      </c>
+      <c r="AW10">
+        <v>48.6</v>
+      </c>
+      <c r="AX10">
+        <v>50.2</v>
+      </c>
+      <c r="AY10">
+        <v>50.5</v>
+      </c>
+      <c r="BF10">
+        <v>51.1</v>
+      </c>
+      <c r="BG10">
+        <v>50.5</v>
+      </c>
+      <c r="BH10">
+        <v>50.9</v>
+      </c>
+      <c r="BI10">
+        <v>50.5</v>
+      </c>
+      <c r="BJ10">
+        <v>51.5</v>
+      </c>
+      <c r="BK10">
+        <v>50.7</v>
+      </c>
+      <c r="BL10">
+        <v>51.5</v>
+      </c>
+      <c r="BM10">
+        <v>50.3</v>
+      </c>
+      <c r="BN10">
+        <v>50.2</v>
+      </c>
+      <c r="BO10">
+        <v>50.9</v>
+      </c>
+      <c r="BP10">
+        <v>49.4</v>
+      </c>
+      <c r="BQ10">
+        <v>47.9</v>
+      </c>
     </row>
-    <row r="11" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>6</v>
       </c>
@@ -1929,8 +2740,68 @@
       <c r="AQ11">
         <v>5.7</v>
       </c>
+      <c r="AR11">
+        <v>46.7</v>
+      </c>
+      <c r="AS11">
+        <v>45.1</v>
+      </c>
+      <c r="AT11">
+        <v>43</v>
+      </c>
+      <c r="AU11">
+        <v>48.9</v>
+      </c>
+      <c r="AV11">
+        <v>44.2</v>
+      </c>
+      <c r="AW11">
+        <v>50.2</v>
+      </c>
+      <c r="AX11">
+        <v>47.4</v>
+      </c>
+      <c r="AY11">
+        <v>52.9</v>
+      </c>
+      <c r="BF11">
+        <v>47.1</v>
+      </c>
+      <c r="BG11">
+        <v>50.8</v>
+      </c>
+      <c r="BH11">
+        <v>46.9</v>
+      </c>
+      <c r="BI11">
+        <v>47.1</v>
+      </c>
+      <c r="BJ11">
+        <v>47.1</v>
+      </c>
+      <c r="BK11">
+        <v>48.3</v>
+      </c>
+      <c r="BL11">
+        <v>49.3</v>
+      </c>
+      <c r="BM11">
+        <v>52.2</v>
+      </c>
+      <c r="BN11">
+        <v>44.2</v>
+      </c>
+      <c r="BO11">
+        <v>49</v>
+      </c>
+      <c r="BP11">
+        <v>48.5</v>
+      </c>
+      <c r="BQ11">
+        <v>47.2</v>
+      </c>
     </row>
-    <row r="12" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>8</v>
       </c>
@@ -2033,8 +2904,68 @@
       <c r="AQ12">
         <v>5.2</v>
       </c>
+      <c r="AR12">
+        <v>46.7</v>
+      </c>
+      <c r="AS12">
+        <v>43.9</v>
+      </c>
+      <c r="AT12">
+        <v>44.6</v>
+      </c>
+      <c r="AU12">
+        <v>43.5</v>
+      </c>
+      <c r="AV12">
+        <v>45.9</v>
+      </c>
+      <c r="AW12">
+        <v>46.7</v>
+      </c>
+      <c r="AX12">
+        <v>46.8</v>
+      </c>
+      <c r="AY12">
+        <v>45.8</v>
+      </c>
+      <c r="BF12">
+        <v>47</v>
+      </c>
+      <c r="BG12">
+        <v>47.8</v>
+      </c>
+      <c r="BH12">
+        <v>47</v>
+      </c>
+      <c r="BI12">
+        <v>45.7</v>
+      </c>
+      <c r="BJ12">
+        <v>45.1</v>
+      </c>
+      <c r="BK12">
+        <v>45.1</v>
+      </c>
+      <c r="BL12">
+        <v>44.4</v>
+      </c>
+      <c r="BM12">
+        <v>46.7</v>
+      </c>
+      <c r="BN12">
+        <v>45</v>
+      </c>
+      <c r="BO12">
+        <v>44.7</v>
+      </c>
+      <c r="BP12">
+        <v>43.9</v>
+      </c>
+      <c r="BQ12">
+        <v>43.2</v>
+      </c>
     </row>
-    <row r="13" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
         <v>8</v>
       </c>
@@ -2146,8 +3077,74 @@
       <c r="AQ13">
         <v>4.2</v>
       </c>
+      <c r="AR13">
+        <v>41.4</v>
+      </c>
+      <c r="AS13">
+        <v>39.9</v>
+      </c>
+      <c r="AT13">
+        <v>38.4</v>
+      </c>
+      <c r="AU13">
+        <v>40.4</v>
+      </c>
+      <c r="AV13">
+        <v>40.5</v>
+      </c>
+      <c r="AW13">
+        <v>41.5</v>
+      </c>
+      <c r="AX13">
+        <v>43.1</v>
+      </c>
+      <c r="AY13">
+        <v>42.6</v>
+      </c>
+      <c r="AZ13">
+        <v>43.4</v>
+      </c>
+      <c r="BA13">
+        <v>43.6</v>
+      </c>
+      <c r="BF13">
+        <v>43.5</v>
+      </c>
+      <c r="BG13">
+        <v>45.2</v>
+      </c>
+      <c r="BH13">
+        <v>44.9</v>
+      </c>
+      <c r="BI13">
+        <v>44.3</v>
+      </c>
+      <c r="BJ13">
+        <v>42.4</v>
+      </c>
+      <c r="BK13">
+        <v>43.9</v>
+      </c>
+      <c r="BL13">
+        <v>43.4</v>
+      </c>
+      <c r="BM13">
+        <v>43.2</v>
+      </c>
+      <c r="BN13">
+        <v>42</v>
+      </c>
+      <c r="BO13">
+        <v>42.2</v>
+      </c>
+      <c r="BP13">
+        <v>41.4</v>
+      </c>
+      <c r="BQ13">
+        <v>43.9</v>
+      </c>
     </row>
-    <row r="14" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -2241,8 +3238,62 @@
       <c r="AQ14">
         <v>5.2</v>
       </c>
+      <c r="AR14">
+        <v>44.3</v>
+      </c>
+      <c r="AS14">
+        <v>42.4</v>
+      </c>
+      <c r="AT14">
+        <v>45.9</v>
+      </c>
+      <c r="AU14">
+        <v>43.9</v>
+      </c>
+      <c r="AV14">
+        <v>46.6</v>
+      </c>
+      <c r="AW14">
+        <v>46</v>
+      </c>
+      <c r="BF14">
+        <v>47.7</v>
+      </c>
+      <c r="BG14">
+        <v>47.7</v>
+      </c>
+      <c r="BH14">
+        <v>48</v>
+      </c>
+      <c r="BI14">
+        <v>48.4</v>
+      </c>
+      <c r="BJ14">
+        <v>46.9</v>
+      </c>
+      <c r="BK14">
+        <v>47.1</v>
+      </c>
+      <c r="BL14">
+        <v>48.6</v>
+      </c>
+      <c r="BM14">
+        <v>48.1</v>
+      </c>
+      <c r="BN14">
+        <v>47.6</v>
+      </c>
+      <c r="BO14">
+        <v>46.9</v>
+      </c>
+      <c r="BP14">
+        <v>45.9</v>
+      </c>
+      <c r="BQ14">
+        <v>45.3</v>
+      </c>
     </row>
-    <row r="15" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
         <v>13</v>
       </c>
@@ -2345,8 +3396,68 @@
       <c r="AQ15">
         <v>5</v>
       </c>
+      <c r="AR15">
+        <v>41.7</v>
+      </c>
+      <c r="AS15">
+        <v>41.9</v>
+      </c>
+      <c r="AT15">
+        <v>42.2</v>
+      </c>
+      <c r="AU15">
+        <v>42.5</v>
+      </c>
+      <c r="AV15">
+        <v>42.8</v>
+      </c>
+      <c r="AW15">
+        <v>44.2</v>
+      </c>
+      <c r="AX15">
+        <v>43.8</v>
+      </c>
+      <c r="AY15">
+        <v>44.8</v>
+      </c>
+      <c r="BF15">
+        <v>43.8</v>
+      </c>
+      <c r="BG15">
+        <v>45</v>
+      </c>
+      <c r="BH15">
+        <v>44.6</v>
+      </c>
+      <c r="BI15">
+        <v>44.2</v>
+      </c>
+      <c r="BJ15">
+        <v>44.4</v>
+      </c>
+      <c r="BK15">
+        <v>43.9</v>
+      </c>
+      <c r="BL15">
+        <v>42.8</v>
+      </c>
+      <c r="BM15">
+        <v>43</v>
+      </c>
+      <c r="BN15">
+        <v>40.6</v>
+      </c>
+      <c r="BO15">
+        <v>43</v>
+      </c>
+      <c r="BP15">
+        <v>41.5</v>
+      </c>
+      <c r="BQ15">
+        <v>41.7</v>
+      </c>
     </row>
-    <row r="16" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>14</v>
       </c>
@@ -2458,8 +3569,74 @@
       <c r="AQ16">
         <v>4.3</v>
       </c>
+      <c r="AR16">
+        <v>47.2</v>
+      </c>
+      <c r="AS16">
+        <v>43.9</v>
+      </c>
+      <c r="AT16">
+        <v>44.7</v>
+      </c>
+      <c r="AU16">
+        <v>43.9</v>
+      </c>
+      <c r="AV16">
+        <v>42.6</v>
+      </c>
+      <c r="AW16">
+        <v>47.7</v>
+      </c>
+      <c r="AX16">
+        <v>44.6</v>
+      </c>
+      <c r="AY16">
+        <v>45.3</v>
+      </c>
+      <c r="AZ16">
+        <v>45.2</v>
+      </c>
+      <c r="BA16">
+        <v>46.9</v>
+      </c>
+      <c r="BF16">
+        <v>48.4</v>
+      </c>
+      <c r="BG16">
+        <v>46.8</v>
+      </c>
+      <c r="BH16">
+        <v>46.4</v>
+      </c>
+      <c r="BI16">
+        <v>46.1</v>
+      </c>
+      <c r="BJ16">
+        <v>45.2</v>
+      </c>
+      <c r="BK16">
+        <v>45.5</v>
+      </c>
+      <c r="BL16">
+        <v>44.7</v>
+      </c>
+      <c r="BM16">
+        <v>45</v>
+      </c>
+      <c r="BN16">
+        <v>42.7</v>
+      </c>
+      <c r="BO16">
+        <v>44.9</v>
+      </c>
+      <c r="BP16">
+        <v>42</v>
+      </c>
+      <c r="BQ16">
+        <v>43.4</v>
+      </c>
     </row>
-    <row r="17" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
         <v>14</v>
       </c>
@@ -2571,8 +3748,74 @@
       <c r="AQ17">
         <v>4.3</v>
       </c>
+      <c r="AR17">
+        <v>46</v>
+      </c>
+      <c r="AS17">
+        <v>43.1</v>
+      </c>
+      <c r="AT17">
+        <v>46.6</v>
+      </c>
+      <c r="AU17">
+        <v>40.9</v>
+      </c>
+      <c r="AV17">
+        <v>47.3</v>
+      </c>
+      <c r="AW17">
+        <v>44.3</v>
+      </c>
+      <c r="AX17">
+        <v>47.6</v>
+      </c>
+      <c r="AY17">
+        <v>44.7</v>
+      </c>
+      <c r="AZ17">
+        <v>47.87364399012516</v>
+      </c>
+      <c r="BA17">
+        <v>47.838633967158295</v>
+      </c>
+      <c r="BF17">
+        <v>49.9</v>
+      </c>
+      <c r="BG17">
+        <v>48.6</v>
+      </c>
+      <c r="BH17">
+        <v>48.2</v>
+      </c>
+      <c r="BI17">
+        <v>50</v>
+      </c>
+      <c r="BJ17">
+        <v>47.6</v>
+      </c>
+      <c r="BK17">
+        <v>45.3</v>
+      </c>
+      <c r="BL17">
+        <v>48.8</v>
+      </c>
+      <c r="BM17">
+        <v>47.5</v>
+      </c>
+      <c r="BN17">
+        <v>46.5</v>
+      </c>
+      <c r="BO17">
+        <v>47.4</v>
+      </c>
+      <c r="BP17">
+        <v>47.1</v>
+      </c>
+      <c r="BQ17">
+        <v>44</v>
+      </c>
     </row>
-    <row r="18" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>15</v>
       </c>
@@ -2675,8 +3918,68 @@
       <c r="AQ18">
         <v>5.3</v>
       </c>
+      <c r="AR18">
+        <v>43.5</v>
+      </c>
+      <c r="AS18">
+        <v>40.1</v>
+      </c>
+      <c r="AT18">
+        <v>44.8</v>
+      </c>
+      <c r="AU18">
+        <v>44.9</v>
+      </c>
+      <c r="AV18">
+        <v>47.5</v>
+      </c>
+      <c r="AW18">
+        <v>45.9</v>
+      </c>
+      <c r="AX18">
+        <v>47.6</v>
+      </c>
+      <c r="AY18">
+        <v>47.7</v>
+      </c>
+      <c r="BF18">
+        <v>46.6</v>
+      </c>
+      <c r="BG18">
+        <v>49.3</v>
+      </c>
+      <c r="BH18">
+        <v>48.7</v>
+      </c>
+      <c r="BI18">
+        <v>48.1</v>
+      </c>
+      <c r="BJ18">
+        <v>47.8</v>
+      </c>
+      <c r="BK18">
+        <v>47.2</v>
+      </c>
+      <c r="BL18">
+        <v>48.2</v>
+      </c>
+      <c r="BM18">
+        <v>47.3</v>
+      </c>
+      <c r="BN18">
+        <v>47.2</v>
+      </c>
+      <c r="BO18">
+        <v>46.6</v>
+      </c>
+      <c r="BP18">
+        <v>45.9</v>
+      </c>
+      <c r="BQ18">
+        <v>45.9</v>
+      </c>
     </row>
-    <row r="19" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:69" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="9">
         <v>15</v>
       </c>
@@ -2779,8 +4082,83 @@
       <c r="AQ19">
         <v>4.8</v>
       </c>
+      <c r="AR19">
+        <v>41.4</v>
+      </c>
+      <c r="AS19">
+        <v>39.6</v>
+      </c>
+      <c r="AT19">
+        <v>42.7</v>
+      </c>
+      <c r="AU19">
+        <v>41</v>
+      </c>
+      <c r="AV19">
+        <v>43.6</v>
+      </c>
+      <c r="AW19">
+        <v>44.3</v>
+      </c>
+      <c r="AX19">
+        <v>46.9</v>
+      </c>
+      <c r="AY19">
+        <v>43.6</v>
+      </c>
+      <c r="BF19">
+        <v>48.1</v>
+      </c>
+      <c r="BG19">
+        <v>47.5</v>
+      </c>
+      <c r="BH19">
+        <v>48.6</v>
+      </c>
+      <c r="BI19">
+        <v>48.4</v>
+      </c>
+      <c r="BJ19">
+        <v>48.3</v>
+      </c>
+      <c r="BK19">
+        <v>47.1</v>
+      </c>
+      <c r="BL19">
+        <v>48.7</v>
+      </c>
+      <c r="BM19">
+        <v>46.5</v>
+      </c>
+      <c r="BN19">
+        <v>45.1</v>
+      </c>
+      <c r="BO19">
+        <v>44.9</v>
+      </c>
+      <c r="BP19">
+        <v>45.6</v>
+      </c>
+      <c r="BQ19">
+        <v>43</v>
+      </c>
     </row>
-    <row r="20" spans="1:43" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:69" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="AS22" s="11"/>
+      <c r="AT22" s="12"/>
+      <c r="AU22" s="12"/>
+      <c r="AV22" s="12"/>
+      <c r="AW22" s="12"/>
+      <c r="AX22" s="12"/>
+      <c r="AY22" s="12"/>
+      <c r="AZ22" s="12"/>
+      <c r="BA22" s="12"/>
+      <c r="BB22" s="12"/>
+      <c r="BC22" s="12"/>
+      <c r="BD22" s="12"/>
+      <c r="BE22" s="13"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>